<commit_message>
alguma coisa mudou ai
</commit_message>
<xml_diff>
--- a/Análise/Levantamento.xlsx
+++ b/Análise/Levantamento.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Documents\Documentos Escola\TCM\BitBucket\organ-web\Análise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8DCE545-4280-46D3-B421-F0E95E7CD081}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B506FBE2-C215-4330-B8E4-5778ED02BE96}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Ecommerce" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,43 +31,16 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Victor</author>
     <author>Milena Monteiro</author>
     <author>tc={EACEF8C7-9F5D-4525-A513-8E7AD2A5A6E9}</author>
     <author>tc={16B91421-E8D3-4A2D-A443-98479880EEF7}</author>
     <author>tc={6C2D57D3-6C94-465C-92CB-FAD0D720BE7B}</author>
     <author>tc={EF8BE035-50E1-4646-B6A1-CA89FE21A62E}</author>
     <author>tc={02088F5B-46C1-4C79-83A6-0D0062579E90}</author>
-    <author>tc={A79DFAC6-A537-43DD-8A68-E30E46360AFD}</author>
     <author>tc={404D62D6-B013-4540-A6BB-D6F85DF28A90}</author>
   </authors>
   <commentList>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{EC847783-9826-4F27-9F9E-4C5644FF9552}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Victor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Email pertence ao cliente ou func
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D8" authorId="1" shapeId="0" xr:uid="{3D866A70-6C5D-4019-A4A4-7DE4409F948D}">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{3D866A70-6C5D-4019-A4A4-7DE4409F948D}">
       <text>
         <r>
           <rPr>
@@ -92,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J8" authorId="2" shapeId="0" xr:uid="{EACEF8C7-9F5D-4525-A513-8E7AD2A5A6E9}">
+    <comment ref="I8" authorId="1" shapeId="0" xr:uid="{EACEF8C7-9F5D-4525-A513-8E7AD2A5A6E9}">
       <text>
         <t>[Comentário encadeado]
 Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
@@ -100,7 +72,7 @@
     QUE MERDA É ESSA</t>
       </text>
     </comment>
-    <comment ref="J13" authorId="3" shapeId="0" xr:uid="{16B91421-E8D3-4A2D-A443-98479880EEF7}">
+    <comment ref="I13" authorId="2" shapeId="0" xr:uid="{16B91421-E8D3-4A2D-A443-98479880EEF7}">
       <text>
         <t>[Comentário encadeado]
 Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
@@ -108,7 +80,7 @@
     Estações ou Safrinha</t>
       </text>
     </comment>
-    <comment ref="H19" authorId="4" shapeId="0" xr:uid="{6C2D57D3-6C94-465C-92CB-FAD0D720BE7B}">
+    <comment ref="H19" authorId="3" shapeId="0" xr:uid="{6C2D57D3-6C94-465C-92CB-FAD0D720BE7B}">
       <text>
         <t>[Comentário encadeado]
 Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
@@ -116,7 +88,7 @@
     Usuários que irão realizar a tarefa</t>
       </text>
     </comment>
-    <comment ref="M19" authorId="5" shapeId="0" xr:uid="{EF8BE035-50E1-4646-B6A1-CA89FE21A62E}">
+    <comment ref="L19" authorId="4" shapeId="0" xr:uid="{EF8BE035-50E1-4646-B6A1-CA89FE21A62E}">
       <text>
         <t>[Comentário encadeado]
 Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
@@ -124,7 +96,7 @@
     Mesma coisa da outra</t>
       </text>
     </comment>
-    <comment ref="P19" authorId="6" shapeId="0" xr:uid="{02088F5B-46C1-4C79-83A6-0D0062579E90}">
+    <comment ref="O19" authorId="5" shapeId="0" xr:uid="{02088F5B-46C1-4C79-83A6-0D0062579E90}">
       <text>
         <t>[Comentário encadeado]
 Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
@@ -132,7 +104,7 @@
     Como criar uma despesa a partir disso?</t>
       </text>
     </comment>
-    <comment ref="F25" authorId="1" shapeId="0" xr:uid="{925102E5-3467-4C2B-BE25-484A56411F78}">
+    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{925102E5-3467-4C2B-BE25-484A56411F78}">
       <text>
         <r>
           <rPr>
@@ -156,15 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J26" authorId="7" shapeId="0" xr:uid="{A79DFAC6-A537-43DD-8A68-E30E46360AFD}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    Mano como funciona isso?</t>
-      </text>
-    </comment>
-    <comment ref="H34" authorId="8" shapeId="0" xr:uid="{404D62D6-B013-4540-A6BB-D6F85DF28A90}">
+    <comment ref="H34" authorId="6" shapeId="0" xr:uid="{404D62D6-B013-4540-A6BB-D6F85DF28A90}">
       <text>
         <t xml:space="preserve">[Comentário encadeado]
 Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
@@ -212,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="229">
   <si>
     <t>Organ - levantamento de dados</t>
   </si>
@@ -241,9 +205,6 @@
     <t>Funcionário</t>
   </si>
   <si>
-    <t>Compra</t>
-  </si>
-  <si>
     <t>Plantio</t>
   </si>
   <si>
@@ -304,9 +265,6 @@
     <t>Título</t>
   </si>
   <si>
-    <t>Código produto</t>
-  </si>
-  <si>
     <t>Nome da Semente</t>
   </si>
   <si>
@@ -352,9 +310,6 @@
     <t>CPF</t>
   </si>
   <si>
-    <t>Código fornecedor</t>
-  </si>
-  <si>
     <t>Código Cultura</t>
   </si>
   <si>
@@ -595,15 +550,9 @@
     <t>Manutenção</t>
   </si>
   <si>
-    <t>Estádio_Especificação</t>
-  </si>
-  <si>
     <t>Estádio</t>
   </si>
   <si>
-    <t>Cultura_Especificação</t>
-  </si>
-  <si>
     <t>Tarefa_Monitoramento</t>
   </si>
   <si>
@@ -637,9 +586,6 @@
     <t>Código estádio</t>
   </si>
   <si>
-    <t>Código cultura</t>
-  </si>
-  <si>
     <t>Parcelas</t>
   </si>
   <si>
@@ -658,9 +604,6 @@
     <t>Código Categoria_produto</t>
   </si>
   <si>
-    <t>Código especificação</t>
-  </si>
-  <si>
     <t>Tempo</t>
   </si>
   <si>
@@ -844,9 +787,6 @@
     <t>classe carrinho, método pra add itens, valor final</t>
   </si>
   <si>
-    <t>Descricao</t>
-  </si>
-  <si>
     <t>É LIDER/ NÃO</t>
   </si>
   <si>
@@ -878,9 +818,6 @@
   </si>
   <si>
     <t>Equipe_Funcionario</t>
-  </si>
-  <si>
-    <t>Especificação</t>
   </si>
   <si>
     <t>CLI/ITEM</t>
@@ -932,7 +869,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1030,24 +967,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1063,15 +982,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="55">
+  <fills count="53">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1206,12 +1118,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1297,12 +1203,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.499984740745262"/>
-        <bgColor rgb="FFE2EFD9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor rgb="FFE2EFD9"/>
       </patternFill>
     </fill>
@@ -1615,7 +1515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1790,86 +1690,95 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="30" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="38" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="40" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="41" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="43" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="44" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="45" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="41" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="42" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="43" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="44" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="45" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="46" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1878,134 +1787,112 @@
     <xf numFmtId="0" fontId="16" fillId="47" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="48" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="49" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="50" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="48" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="51" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="52" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="53" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="54" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="39" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="42" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="45" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="51" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="41" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="51" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="51" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="52" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="51" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="52" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="40" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="43" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="49" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="49" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="49" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="49" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="50" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2016,6 +1903,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2355,23 +2251,20 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="J8" dT="2019-08-03T19:31:26.79" personId="{A3130C86-08E9-46CA-B8B9-B8B6DCCC2259}" id="{EACEF8C7-9F5D-4525-A513-8E7AD2A5A6E9}">
+  <threadedComment ref="I8" dT="2019-08-03T19:31:26.79" personId="{A3130C86-08E9-46CA-B8B9-B8B6DCCC2259}" id="{EACEF8C7-9F5D-4525-A513-8E7AD2A5A6E9}">
     <text>QUE MERDA É ESSA</text>
   </threadedComment>
-  <threadedComment ref="J13" dT="2019-07-26T20:12:28.26" personId="{CCB6A4E5-3869-4749-843A-36CD6CFF6E51}" id="{16B91421-E8D3-4A2D-A443-98479880EEF7}">
+  <threadedComment ref="I13" dT="2019-07-26T20:12:28.26" personId="{CCB6A4E5-3869-4749-843A-36CD6CFF6E51}" id="{16B91421-E8D3-4A2D-A443-98479880EEF7}">
     <text>Estações ou Safrinha</text>
   </threadedComment>
   <threadedComment ref="H19" dT="2019-07-25T22:00:31.58" personId="{CCB6A4E5-3869-4749-843A-36CD6CFF6E51}" id="{6C2D57D3-6C94-465C-92CB-FAD0D720BE7B}">
     <text>Usuários que irão realizar a tarefa</text>
   </threadedComment>
-  <threadedComment ref="M19" dT="2019-08-01T00:36:57.07" personId="{A3130C86-08E9-46CA-B8B9-B8B6DCCC2259}" id="{EF8BE035-50E1-4646-B6A1-CA89FE21A62E}">
+  <threadedComment ref="L19" dT="2019-08-01T00:36:57.07" personId="{A3130C86-08E9-46CA-B8B9-B8B6DCCC2259}" id="{EF8BE035-50E1-4646-B6A1-CA89FE21A62E}">
     <text>Mesma coisa da outra</text>
   </threadedComment>
-  <threadedComment ref="P19" dT="2019-07-27T00:48:39.04" personId="{CCB6A4E5-3869-4749-843A-36CD6CFF6E51}" id="{02088F5B-46C1-4C79-83A6-0D0062579E90}">
+  <threadedComment ref="O19" dT="2019-07-27T00:48:39.04" personId="{CCB6A4E5-3869-4749-843A-36CD6CFF6E51}" id="{02088F5B-46C1-4C79-83A6-0D0062579E90}">
     <text>Como criar uma despesa a partir disso?</text>
-  </threadedComment>
-  <threadedComment ref="J26" dT="2019-08-01T00:17:02.80" personId="{A3130C86-08E9-46CA-B8B9-B8B6DCCC2259}" id="{A79DFAC6-A537-43DD-8A68-E30E46360AFD}">
-    <text>Mano como funciona isso?</text>
   </threadedComment>
   <threadedComment ref="H34" dT="2019-07-26T22:11:40.47" personId="{A3130C86-08E9-46CA-B8B9-B8B6DCCC2259}" id="{404D62D6-B013-4540-A6BB-D6F85DF28A90}">
     <text xml:space="preserve">Opcional. Ex.: Fixo, Pessoal, Empresa, Da Mãe
@@ -2382,10 +2275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI1000"/>
+  <dimension ref="A1:AH1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D9"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2398,68 +2291,66 @@
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" customWidth="1"/>
-    <col min="16" max="16" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.140625" customWidth="1"/>
-    <col min="23" max="23" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.85546875" customWidth="1"/>
-    <col min="26" max="26" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" customWidth="1"/>
+    <col min="15" max="15" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.140625" customWidth="1"/>
+    <col min="22" max="22" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.85546875" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
+    <row r="1" spans="1:34" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="145"/>
-      <c r="K1" s="145"/>
-      <c r="L1" s="145"/>
-      <c r="M1" s="145"/>
-      <c r="N1" s="145"/>
-      <c r="O1" s="145"/>
-      <c r="P1" s="145"/>
-      <c r="Q1" s="145"/>
-      <c r="R1" s="145"/>
-      <c r="S1" s="145"/>
-      <c r="T1" s="145"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="144" t="s">
-        <v>229</v>
-      </c>
-      <c r="W1" s="144"/>
-      <c r="X1" s="144"/>
-      <c r="Y1" s="144"/>
-      <c r="Z1" s="144"/>
-      <c r="AA1" s="144"/>
-      <c r="AB1" s="144"/>
-      <c r="AC1" s="144"/>
-      <c r="AD1" s="144"/>
-      <c r="AE1" s="144"/>
-      <c r="AF1" s="144"/>
-      <c r="AG1" s="144"/>
-      <c r="AH1" s="144"/>
-      <c r="AI1" s="144"/>
-    </row>
-    <row r="2" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="140"/>
+      <c r="K1" s="140"/>
+      <c r="L1" s="140"/>
+      <c r="M1" s="140"/>
+      <c r="N1" s="140"/>
+      <c r="O1" s="140"/>
+      <c r="P1" s="140"/>
+      <c r="Q1" s="140"/>
+      <c r="R1" s="140"/>
+      <c r="S1" s="140"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="139" t="s">
+        <v>220</v>
+      </c>
+      <c r="V1" s="139"/>
+      <c r="W1" s="139"/>
+      <c r="X1" s="139"/>
+      <c r="Y1" s="139"/>
+      <c r="Z1" s="139"/>
+      <c r="AA1" s="139"/>
+      <c r="AB1" s="139"/>
+      <c r="AC1" s="139"/>
+      <c r="AD1" s="139"/>
+      <c r="AE1" s="139"/>
+      <c r="AF1" s="139"/>
+      <c r="AG1" s="139"/>
+      <c r="AH1" s="139"/>
+    </row>
+    <row r="2" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
         <v>1</v>
       </c>
@@ -2476,7 +2367,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="85" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="G2" s="88" t="s">
         <v>7</v>
@@ -2484,535 +2375,511 @@
       <c r="H2" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="112" t="s">
+      <c r="I2" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="91" t="s">
+      <c r="J2" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="94" t="s">
+      <c r="K2" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="95" t="s">
+      <c r="L2" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="99" t="s">
+      <c r="M2" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="102" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="105" t="s">
+      <c r="N2" s="105" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="74" t="s">
+      <c r="P2" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="77" t="s">
-        <v>18</v>
-      </c>
-      <c r="R2" s="111" t="s">
+      <c r="Q2" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="110" t="s">
+      <c r="S2" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="109" t="s">
+      <c r="U2" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+    </row>
+    <row r="3" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="40" t="s">
-        <v>215</v>
-      </c>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-    </row>
-    <row r="3" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
-        <v>23</v>
-      </c>
       <c r="B3" s="76" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="78" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="82" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="125" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="124" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="123" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="122" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="113" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="121" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="93" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="96" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="103" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" s="106" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" s="107" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" s="108" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="121" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="120" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="119" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="118" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="93" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="96" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="103" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="106" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="107" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="108" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="U3" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
+    </row>
+    <row r="4" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="T3" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="V3" s="41" t="s">
-        <v>231</v>
-      </c>
-      <c r="W3" s="30"/>
-      <c r="X3" s="30"/>
-    </row>
-    <row r="4" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="70" t="s">
+      <c r="B4" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="C4" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="82" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="87" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="78" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="82" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="83" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="14" t="s">
+      <c r="K4" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="87" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="113" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="93" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" s="96" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="103" t="s">
+      <c r="L4" s="96" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="103" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="106" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="137" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="P4" s="106" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="142" t="s">
-        <v>27</v>
-      </c>
-      <c r="R4" s="108" t="s">
+      <c r="R4" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="S4" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" s="41" t="s">
+        <v>205</v>
+      </c>
+      <c r="V4" s="30"/>
+      <c r="W4" s="30"/>
+    </row>
+    <row r="5" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="S4" s="38" t="s">
-        <v>233</v>
-      </c>
-      <c r="T4" s="39" t="s">
+      <c r="B5" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="V4" s="41" t="s">
-        <v>213</v>
-      </c>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-    </row>
-    <row r="5" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="70" t="s">
+      <c r="C5" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="76" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="78" t="s">
-        <v>40</v>
-      </c>
       <c r="D5" s="82" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="87" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="87" t="s">
+      <c r="I5" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="35" t="s">
+      <c r="J5" s="93" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="113" t="s">
+      <c r="L5" s="96" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="120" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" s="93" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="33" t="s">
+      <c r="N5" s="104" t="s">
         <v>48</v>
       </c>
-      <c r="M5" s="96" t="s">
-        <v>43</v>
-      </c>
-      <c r="N5" s="128" t="s">
+      <c r="O5" s="106" t="s">
         <v>49</v>
       </c>
-      <c r="O5" s="104" t="s">
-        <v>51</v>
-      </c>
-      <c r="P5" s="106" t="s">
+      <c r="P5" s="127" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q5" s="138" t="s">
+        <v>228</v>
+      </c>
+      <c r="R5" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="Q5" s="131" t="s">
-        <v>90</v>
-      </c>
-      <c r="R5" s="143" t="s">
-        <v>237</v>
-      </c>
-      <c r="S5" s="38" t="s">
+      <c r="S5" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="U5" s="41" t="s">
+        <v>206</v>
+      </c>
+      <c r="V5" s="30"/>
+      <c r="W5" s="30"/>
+    </row>
+    <row r="6" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="70" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="133" t="s">
         <v>55</v>
       </c>
-      <c r="T5" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="V5" s="41" t="s">
-        <v>214</v>
-      </c>
-      <c r="W5" s="30"/>
-      <c r="X5" s="30"/>
-    </row>
-    <row r="6" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="70" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="76" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="138" t="s">
-        <v>58</v>
-      </c>
       <c r="D6" s="82" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="122" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="96" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" s="15"/>
+      <c r="O6" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="87" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="I6" s="113" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" s="126" t="s">
-        <v>63</v>
-      </c>
-      <c r="L6" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="M6" s="96" t="s">
-        <v>65</v>
-      </c>
-      <c r="N6" s="37" t="s">
+      <c r="P6" s="107" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="O6" s="15"/>
-      <c r="P6" s="106" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q6" s="107" t="s">
-        <v>43</v>
-      </c>
-      <c r="R6" s="108" t="s">
-        <v>69</v>
-      </c>
-      <c r="S6" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="T6" s="39" t="s">
-        <v>27</v>
-      </c>
+      <c r="R6" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="S6" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="T6" s="30"/>
       <c r="U6" s="30"/>
       <c r="V6" s="30"/>
       <c r="W6" s="30"/>
-      <c r="X6" s="30"/>
-    </row>
-    <row r="7" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="76" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>220</v>
-      </c>
-      <c r="D7" s="135" t="s">
-        <v>85</v>
+        <v>212</v>
+      </c>
+      <c r="D7" s="82" t="s">
+        <v>92</v>
       </c>
       <c r="F7" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="87" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="87" t="s">
+      <c r="J7" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="K7" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7" s="123" t="s">
+        <v>74</v>
+      </c>
+      <c r="M7" s="124" t="s">
+        <v>76</v>
+      </c>
+      <c r="N7" s="15"/>
+      <c r="O7" s="106" t="s">
+        <v>78</v>
+      </c>
+      <c r="P7" s="127" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q7" s="108" t="s">
+        <v>80</v>
+      </c>
+      <c r="R7" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="S7" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="113" t="s">
-        <v>73</v>
-      </c>
-      <c r="J7" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="K7" s="93" t="s">
-        <v>75</v>
-      </c>
-      <c r="L7" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="M7" s="127" t="s">
-        <v>77</v>
-      </c>
-      <c r="N7" s="128" t="s">
-        <v>79</v>
-      </c>
-      <c r="O7" s="15"/>
-      <c r="P7" s="106" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q7" s="131" t="s">
-        <v>73</v>
-      </c>
-      <c r="R7" s="108" t="s">
-        <v>83</v>
-      </c>
-      <c r="S7" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="T7" s="39" t="s">
-        <v>43</v>
-      </c>
+      <c r="T7" s="30"/>
       <c r="U7" s="30"/>
       <c r="V7" s="30"/>
       <c r="W7" s="30"/>
-      <c r="X7" s="30"/>
-    </row>
-    <row r="8" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="15"/>
       <c r="C8" s="18"/>
       <c r="D8" s="82" t="s">
-        <v>95</v>
+        <v>223</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="87" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="K8" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="87" t="s">
+      <c r="L8" s="123" t="s">
+        <v>227</v>
+      </c>
+      <c r="M8" s="37"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="106" t="s">
+        <v>88</v>
+      </c>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="108" t="s">
+        <v>90</v>
+      </c>
+      <c r="R8" s="15"/>
+      <c r="S8" s="129" t="s">
         <v>87</v>
       </c>
-      <c r="H8" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="114"/>
-      <c r="J8" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="K8" s="15"/>
-      <c r="L8" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="M8" s="127" t="s">
-        <v>236</v>
-      </c>
-      <c r="N8" s="37"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="106" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="108" t="s">
-        <v>93</v>
-      </c>
-      <c r="S8" s="15"/>
-      <c r="T8" s="133" t="s">
-        <v>90</v>
-      </c>
+      <c r="T8" s="30"/>
       <c r="U8" s="30"/>
       <c r="V8" s="30"/>
       <c r="W8" s="30"/>
-      <c r="X8" s="30"/>
-    </row>
-    <row r="9" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
-      <c r="D9" s="82" t="s">
-        <v>232</v>
-      </c>
+      <c r="D9" s="18"/>
       <c r="E9" s="18"/>
-      <c r="F9" s="117" t="s">
-        <v>217</v>
+      <c r="F9" s="113" t="s">
+        <v>209</v>
       </c>
       <c r="G9" s="87" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="I9" s="114"/>
-      <c r="J9" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="130" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" s="15"/>
+      <c r="M9" s="124" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="15"/>
+      <c r="O9" s="106" t="s">
+        <v>94</v>
+      </c>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="108" t="s">
         <v>96</v>
       </c>
-      <c r="K9" s="15"/>
-      <c r="L9" s="134" t="s">
-        <v>63</v>
-      </c>
-      <c r="M9" s="15"/>
-      <c r="N9" s="128" t="s">
-        <v>49</v>
-      </c>
-      <c r="O9" s="15"/>
-      <c r="P9" s="106" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="108" t="s">
-        <v>99</v>
-      </c>
+      <c r="R9" s="15"/>
       <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
+      <c r="T9" s="30"/>
       <c r="U9" s="30"/>
       <c r="V9" s="30"/>
       <c r="W9" s="30"/>
-      <c r="X9" s="30"/>
-    </row>
-    <row r="10" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
       <c r="F10" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="G10" s="118" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" s="114" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10" s="115" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="K10" s="130" t="s">
         <v>100</v>
       </c>
-      <c r="H10" s="119" t="s">
+      <c r="L10" s="15"/>
+      <c r="M10" s="100" t="s">
+        <v>212</v>
+      </c>
+      <c r="N10" s="19"/>
+      <c r="O10" s="106" t="s">
         <v>101</v>
       </c>
-      <c r="I10" s="114"/>
-      <c r="J10" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="134" t="s">
-        <v>103</v>
-      </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="100" t="s">
-        <v>220</v>
-      </c>
-      <c r="O10" s="19"/>
-      <c r="P10" s="106" t="s">
-        <v>104</v>
-      </c>
+      <c r="P10" s="18"/>
       <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="15"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="30"/>
       <c r="U10" s="30"/>
       <c r="V10" s="30"/>
       <c r="W10" s="30"/>
-      <c r="X10" s="30"/>
-    </row>
-    <row r="11" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
       <c r="F11" s="14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G11" s="87" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H11" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="I11" s="114"/>
-      <c r="J11" s="120" t="s">
-        <v>107</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="I11" s="116" t="s">
+        <v>104</v>
+      </c>
+      <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
+      <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="106" t="s">
-        <v>108</v>
-      </c>
+      <c r="O11" s="106" t="s">
+        <v>105</v>
+      </c>
+      <c r="P11" s="15"/>
       <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="15"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="30"/>
       <c r="U11" s="30"/>
       <c r="V11" s="30"/>
       <c r="W11" s="30"/>
-      <c r="X11" s="30"/>
-    </row>
-    <row r="12" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="15"/>
       <c r="C12" s="31"/>
@@ -3020,59 +2887,57 @@
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="18"/>
-      <c r="H12" s="119" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="114"/>
-      <c r="J12" s="36" t="s">
-        <v>110</v>
-      </c>
+      <c r="H12" s="115" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="J12" s="15"/>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="12"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="30"/>
       <c r="U12" s="30"/>
       <c r="V12" s="30"/>
       <c r="W12" s="30"/>
-      <c r="X12" s="30"/>
-    </row>
-    <row r="13" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="72"/>
       <c r="B13" s="31"/>
       <c r="C13" s="22"/>
-      <c r="D13" s="18"/>
+      <c r="D13" s="15"/>
       <c r="E13" s="18"/>
       <c r="F13" s="12"/>
       <c r="G13" s="15"/>
       <c r="H13" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="I13" s="114"/>
-      <c r="J13" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="K13" s="18"/>
+        <v>108</v>
+      </c>
+      <c r="I13" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="J13" s="18"/>
+      <c r="K13" s="15"/>
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="15"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="12"/>
       <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
+      <c r="T13" s="30"/>
       <c r="U13" s="30"/>
       <c r="V13" s="30"/>
       <c r="W13" s="30"/>
-      <c r="X13" s="30"/>
-    </row>
-    <row r="14" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
       <c r="B14" s="22"/>
       <c r="C14" s="18"/>
@@ -3081,28 +2946,27 @@
       <c r="F14" s="12"/>
       <c r="G14" s="15"/>
       <c r="H14" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I14" s="114"/>
-      <c r="J14" s="36" t="s">
-        <v>114</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="I14" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="J14" s="18"/>
       <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
+      <c r="L14" s="15"/>
       <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="18"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="15"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="30"/>
       <c r="U14" s="30"/>
       <c r="V14" s="30"/>
       <c r="W14" s="30"/>
-      <c r="X14" s="30"/>
-    </row>
-    <row r="15" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="15"/>
       <c r="C15" s="18"/>
@@ -3111,26 +2975,25 @@
       <c r="F15" s="12"/>
       <c r="G15" s="15"/>
       <c r="H15" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="I15" s="114"/>
-      <c r="J15" s="15"/>
+        <v>112</v>
+      </c>
+      <c r="I15" s="15"/>
+      <c r="J15" s="18"/>
       <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
+      <c r="L15" s="15"/>
       <c r="M15" s="15"/>
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="15"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="30"/>
       <c r="U15" s="30"/>
       <c r="V15" s="30"/>
       <c r="W15" s="30"/>
-      <c r="X15" s="30"/>
-    </row>
-    <row r="16" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="15"/>
       <c r="C16" s="18"/>
@@ -3139,54 +3002,52 @@
       <c r="F16" s="20"/>
       <c r="G16" s="15"/>
       <c r="H16" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="I16" s="114"/>
-      <c r="J16" s="15"/>
+        <v>113</v>
+      </c>
+      <c r="I16" s="15"/>
+      <c r="J16" s="18"/>
       <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
+      <c r="L16" s="15"/>
       <c r="M16" s="15"/>
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
       <c r="P16" s="15"/>
       <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="15"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="30"/>
       <c r="U16" s="30"/>
       <c r="V16" s="30"/>
       <c r="W16" s="30"/>
-      <c r="X16" s="30"/>
-    </row>
-    <row r="17" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="15"/>
       <c r="C17" s="18"/>
-      <c r="D17" s="15"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="20"/>
       <c r="F17" s="15"/>
       <c r="G17" s="20"/>
-      <c r="H17" s="119" t="s">
-        <v>117</v>
-      </c>
-      <c r="I17" s="114"/>
+      <c r="H17" s="115" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="21"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="15"/>
       <c r="R17" s="15"/>
       <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
+      <c r="T17" s="30"/>
       <c r="U17" s="30"/>
       <c r="V17" s="30"/>
       <c r="W17" s="30"/>
-      <c r="X17" s="30"/>
-    </row>
-    <row r="18" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="15"/>
       <c r="C18" s="12"/>
@@ -3195,26 +3056,25 @@
       <c r="F18" s="12"/>
       <c r="G18" s="15"/>
       <c r="H18" s="18"/>
-      <c r="I18" s="115"/>
+      <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="18"/>
       <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="12"/>
-      <c r="T18" s="15"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="30"/>
       <c r="U18" s="30"/>
       <c r="V18" s="30"/>
       <c r="W18" s="30"/>
-      <c r="X18" s="30"/>
-    </row>
-    <row r="19" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="75" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B19" s="77" t="s">
         <v>2</v>
@@ -3222,231 +3082,226 @@
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="84" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="F19" s="34" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G19" s="12"/>
       <c r="H19" s="89" t="s">
-        <v>218</v>
-      </c>
-      <c r="I19" s="12"/>
-      <c r="J19" s="92" t="s">
-        <v>128</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="I19" s="92" t="s">
+        <v>124</v>
+      </c>
+      <c r="J19" s="12"/>
       <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="98" t="s">
-        <v>53</v>
-      </c>
-      <c r="N19" s="101" t="s">
-        <v>124</v>
-      </c>
-      <c r="O19" s="105" t="s">
-        <v>15</v>
-      </c>
-      <c r="P19" s="75" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q19" s="139" t="s">
-        <v>118</v>
-      </c>
-      <c r="R19" s="12"/>
-      <c r="S19" s="110" t="s">
-        <v>130</v>
-      </c>
-      <c r="T19" s="12"/>
+      <c r="L19" s="98" t="s">
+        <v>50</v>
+      </c>
+      <c r="M19" s="101" t="s">
+        <v>121</v>
+      </c>
+      <c r="N19" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="O19" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="P19" s="134" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="110" t="s">
+        <v>125</v>
+      </c>
+      <c r="S19" s="12"/>
+      <c r="T19" s="30"/>
       <c r="U19" s="30"/>
       <c r="V19" s="30"/>
       <c r="W19" s="30"/>
-      <c r="X19" s="30"/>
-    </row>
-    <row r="20" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="137" t="s">
-        <v>234</v>
+        <v>22</v>
+      </c>
+      <c r="B20" s="132" t="s">
+        <v>225</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="12"/>
       <c r="H20" s="35"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="121" t="s">
+      <c r="I20" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="97" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="97" t="s">
-        <v>23</v>
-      </c>
-      <c r="N20" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="O20" s="129" t="s">
-        <v>24</v>
-      </c>
-      <c r="P20" s="106" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q20" s="140" t="s">
-        <v>23</v>
-      </c>
-      <c r="R20" s="12"/>
-      <c r="S20" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="T20" s="12"/>
+      <c r="O20" s="106" t="s">
+        <v>22</v>
+      </c>
+      <c r="P20" s="135" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="S20" s="12"/>
+      <c r="T20" s="30"/>
       <c r="U20" s="30"/>
       <c r="V20" s="30"/>
       <c r="W20" s="30"/>
-      <c r="X20" s="30"/>
-    </row>
-    <row r="21" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="137" t="s">
-        <v>235</v>
+        <v>39</v>
+      </c>
+      <c r="B21" s="132" t="s">
+        <v>226</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="116" t="s">
-        <v>133</v>
-      </c>
-      <c r="F21" s="117" t="s">
-        <v>137</v>
+      <c r="D21" s="15"/>
+      <c r="E21" s="112" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" s="113" t="s">
+        <v>132</v>
       </c>
       <c r="G21" s="12"/>
-      <c r="H21" s="119" t="s">
-        <v>135</v>
-      </c>
-      <c r="I21" s="12"/>
-      <c r="J21" s="36" t="s">
-        <v>27</v>
-      </c>
+      <c r="H21" s="115" t="s">
+        <v>130</v>
+      </c>
+      <c r="I21" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="12"/>
       <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="97" t="s">
-        <v>27</v>
-      </c>
-      <c r="N21" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="O21" s="103" t="s">
-        <v>33</v>
-      </c>
-      <c r="P21" s="106" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q21" s="140" t="s">
-        <v>131</v>
-      </c>
-      <c r="R21" s="12"/>
-      <c r="S21" s="132" t="s">
-        <v>135</v>
-      </c>
-      <c r="T21" s="12"/>
+      <c r="L21" s="97" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21" s="103" t="s">
+        <v>31</v>
+      </c>
+      <c r="O21" s="106" t="s">
+        <v>26</v>
+      </c>
+      <c r="P21" s="135" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="128" t="s">
+        <v>130</v>
+      </c>
+      <c r="S21" s="12"/>
+      <c r="T21" s="30"/>
       <c r="U21" s="30"/>
       <c r="V21" s="30"/>
       <c r="W21" s="30"/>
-      <c r="X21" s="30"/>
-    </row>
-    <row r="22" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="71" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="116" t="s">
-        <v>171</v>
-      </c>
-      <c r="F22" s="117" t="s">
-        <v>145</v>
+      <c r="E22" s="112" t="s">
+        <v>164</v>
+      </c>
+      <c r="F22" s="113" t="s">
+        <v>139</v>
       </c>
       <c r="G22" s="12"/>
-      <c r="H22" s="119" t="s">
-        <v>219</v>
-      </c>
-      <c r="I22" s="12"/>
-      <c r="J22" s="36" t="s">
-        <v>149</v>
-      </c>
-      <c r="K22" s="15"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="97" t="s">
-        <v>212</v>
-      </c>
-      <c r="N22" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="O22" s="103" t="s">
-        <v>50</v>
-      </c>
-      <c r="P22" s="106" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q22" s="140" t="s">
+      <c r="H22" s="115" t="s">
+        <v>211</v>
+      </c>
+      <c r="I22" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="R22" s="12"/>
-      <c r="S22" s="132" t="s">
-        <v>150</v>
-      </c>
-      <c r="T22" s="12"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="97" t="s">
+        <v>204</v>
+      </c>
+      <c r="M22" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="N22" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="O22" s="106" t="s">
+        <v>27</v>
+      </c>
+      <c r="P22" s="135" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="128" t="s">
+        <v>143</v>
+      </c>
+      <c r="S22" s="12"/>
+      <c r="T22" s="30"/>
       <c r="U22" s="30"/>
       <c r="V22" s="30"/>
       <c r="W22" s="30"/>
-      <c r="X22" s="30"/>
-    </row>
-    <row r="23" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="71" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="18"/>
-      <c r="D23" s="15"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="86" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F23" s="18"/>
       <c r="G23" s="12"/>
       <c r="H23" s="18"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="K23" s="15"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="O23" s="103" t="s">
-        <v>67</v>
-      </c>
-      <c r="P23" s="130"/>
-      <c r="Q23" s="141" t="s">
-        <v>34</v>
-      </c>
+      <c r="I23" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="J23" s="15"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="N23" s="103" t="s">
+        <v>64</v>
+      </c>
+      <c r="O23" s="126"/>
+      <c r="P23" s="136" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q23" s="12"/>
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
-      <c r="T23" s="12"/>
+      <c r="T23" s="30"/>
       <c r="U23" s="30"/>
       <c r="V23" s="30"/>
       <c r="W23" s="30"/>
-      <c r="X23" s="30"/>
-    </row>
-    <row r="24" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="136" t="s">
-        <v>140</v>
+    </row>
+    <row r="24" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="131" t="s">
+        <v>135</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="12"/>
@@ -3455,65 +3310,65 @@
       <c r="G24" s="12"/>
       <c r="H24" s="18"/>
       <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="15"/>
       <c r="L24" s="15"/>
       <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="103" t="s">
-        <v>80</v>
-      </c>
-      <c r="P24" s="106" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q24" s="141" t="s">
-        <v>153</v>
-      </c>
+      <c r="N24" s="103" t="s">
+        <v>77</v>
+      </c>
+      <c r="O24" s="106" t="s">
+        <v>145</v>
+      </c>
+      <c r="P24" s="136" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q24" s="12"/>
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
-      <c r="T24" s="12"/>
+      <c r="T24" s="30"/>
       <c r="U24" s="30"/>
       <c r="V24" s="30"/>
       <c r="W24" s="30"/>
-      <c r="X24" s="30"/>
-    </row>
-    <row r="25" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="70" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="34" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="89" t="s">
-        <v>169</v>
-      </c>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
+        <v>162</v>
+      </c>
+      <c r="I25" s="92" t="s">
+        <v>120</v>
+      </c>
+      <c r="J25" s="18"/>
       <c r="K25" s="18"/>
       <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="104" t="s">
-        <v>51</v>
-      </c>
-      <c r="P25" s="18"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="O25" s="18"/>
+      <c r="P25" s="12"/>
       <c r="Q25" s="12"/>
       <c r="R25" s="12"/>
       <c r="S25" s="12"/>
-      <c r="T25" s="12"/>
+      <c r="T25" s="30"/>
       <c r="U25" s="30"/>
       <c r="V25" s="30"/>
       <c r="W25" s="30"/>
-      <c r="X25" s="30"/>
-    </row>
-    <row r="26" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="70" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -3521,99 +3376,96 @@
       <c r="E26" s="12"/>
       <c r="F26" s="14"/>
       <c r="G26" s="12"/>
-      <c r="H26" s="119" t="s">
-        <v>163</v>
-      </c>
-      <c r="I26" s="12"/>
-      <c r="J26" s="92" t="s">
-        <v>222</v>
-      </c>
+      <c r="H26" s="115" t="s">
+        <v>156</v>
+      </c>
+      <c r="I26" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="18"/>
       <c r="K26" s="18"/>
       <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="101" t="s">
-        <v>121</v>
-      </c>
+      <c r="M26" s="101" t="s">
+        <v>118</v>
+      </c>
+      <c r="N26" s="18"/>
       <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
+      <c r="P26" s="12"/>
       <c r="Q26" s="12"/>
       <c r="R26" s="12"/>
       <c r="S26" s="12"/>
-      <c r="T26" s="12"/>
+      <c r="T26" s="30"/>
       <c r="U26" s="30"/>
       <c r="V26" s="30"/>
       <c r="W26" s="30"/>
-      <c r="X26" s="30"/>
-    </row>
-    <row r="27" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="73"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
+      <c r="D27" s="16"/>
       <c r="E27" s="12"/>
-      <c r="F27" s="117" t="s">
-        <v>135</v>
+      <c r="F27" s="113" t="s">
+        <v>130</v>
       </c>
       <c r="G27" s="12"/>
-      <c r="H27" s="119" t="s">
-        <v>171</v>
-      </c>
-      <c r="I27" s="12"/>
-      <c r="J27" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="K27" s="15"/>
+      <c r="H27" s="115" t="s">
+        <v>164</v>
+      </c>
+      <c r="I27" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="J27" s="15"/>
+      <c r="K27" s="18"/>
       <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="75" t="s">
-        <v>164</v>
-      </c>
+      <c r="M27" s="37"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="P27" s="12"/>
       <c r="Q27" s="12"/>
       <c r="R27" s="12"/>
       <c r="S27" s="12"/>
-      <c r="T27" s="12"/>
+      <c r="T27" s="30"/>
       <c r="U27" s="30"/>
       <c r="V27" s="30"/>
       <c r="W27" s="30"/>
-      <c r="X27" s="30"/>
-    </row>
-    <row r="28" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="73"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="16"/>
       <c r="E28" s="12"/>
-      <c r="F28" s="117" t="s">
-        <v>144</v>
+      <c r="F28" s="113" t="s">
+        <v>138</v>
       </c>
       <c r="G28" s="12"/>
       <c r="H28" s="15"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="36" t="s">
-        <v>210</v>
-      </c>
+      <c r="I28" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="J28" s="15"/>
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="128" t="s">
-        <v>136</v>
-      </c>
-      <c r="O28" s="15"/>
-      <c r="P28" s="106"/>
+      <c r="M28" s="124" t="s">
+        <v>131</v>
+      </c>
+      <c r="N28" s="15"/>
+      <c r="O28" s="106"/>
+      <c r="P28" s="12"/>
       <c r="Q28" s="12"/>
       <c r="R28" s="12"/>
       <c r="S28" s="12"/>
-      <c r="T28" s="12"/>
+      <c r="T28" s="30"/>
       <c r="U28" s="30"/>
       <c r="V28" s="30"/>
       <c r="W28" s="30"/>
-      <c r="X28" s="30"/>
-    </row>
-    <row r="29" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="75" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="12"/>
@@ -3622,28 +3474,27 @@
       <c r="F29" s="18"/>
       <c r="G29" s="12"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="12"/>
+      <c r="I29" s="15"/>
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="128" t="s">
-        <v>145</v>
-      </c>
-      <c r="O29" s="15"/>
-      <c r="P29" s="130" t="s">
-        <v>160</v>
-      </c>
+      <c r="M29" s="124" t="s">
+        <v>139</v>
+      </c>
+      <c r="N29" s="15"/>
+      <c r="O29" s="126" t="s">
+        <v>153</v>
+      </c>
+      <c r="P29" s="12"/>
       <c r="Q29" s="12"/>
       <c r="R29" s="12"/>
       <c r="S29" s="12"/>
-      <c r="T29" s="12"/>
+      <c r="T29" s="30"/>
       <c r="U29" s="30"/>
       <c r="V29" s="30"/>
       <c r="W29" s="30"/>
-      <c r="X29" s="30"/>
-    </row>
-    <row r="30" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="70"/>
       <c r="B30" s="16"/>
       <c r="C30" s="12"/>
@@ -3652,90 +3503,85 @@
       <c r="F30" s="18"/>
       <c r="G30" s="15"/>
       <c r="H30" s="89" t="s">
-        <v>72</v>
-      </c>
-      <c r="I30" s="12"/>
+        <v>69</v>
+      </c>
+      <c r="I30" s="15"/>
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="130" t="s">
-        <v>167</v>
-      </c>
+      <c r="M30" s="12"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="126" t="s">
+        <v>160</v>
+      </c>
+      <c r="P30" s="12"/>
       <c r="Q30" s="12"/>
       <c r="R30" s="12"/>
       <c r="S30" s="12"/>
-      <c r="T30" s="12"/>
+      <c r="T30" s="30"/>
       <c r="U30" s="30"/>
       <c r="V30" s="30"/>
       <c r="W30" s="30"/>
-      <c r="X30" s="30"/>
-    </row>
-    <row r="31" spans="1:24" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="136" t="s">
-        <v>161</v>
+    </row>
+    <row r="31" spans="1:23" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="131" t="s">
+        <v>154</v>
       </c>
       <c r="B31" s="16"/>
       <c r="C31" s="12"/>
-      <c r="D31" s="16"/>
+      <c r="D31" s="15"/>
       <c r="E31" s="16"/>
       <c r="F31" s="18"/>
       <c r="G31" s="12"/>
-      <c r="H31" s="122" t="s">
-        <v>23</v>
-      </c>
-      <c r="I31" s="15"/>
-      <c r="J31" s="92" t="s">
-        <v>127</v>
-      </c>
+      <c r="H31" s="118" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="144"/>
+      <c r="J31" s="15"/>
       <c r="K31" s="15"/>
       <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="15"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="12"/>
       <c r="P31" s="12"/>
       <c r="Q31" s="12"/>
       <c r="R31" s="12"/>
       <c r="S31" s="12"/>
-      <c r="T31" s="12"/>
+      <c r="T31" s="30"/>
       <c r="U31" s="30"/>
       <c r="V31" s="30"/>
       <c r="W31" s="30"/>
-      <c r="X31" s="30"/>
-    </row>
-    <row r="32" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="136" t="s">
-        <v>165</v>
+    </row>
+    <row r="32" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="131" t="s">
+        <v>158</v>
       </c>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
-      <c r="D32" s="15"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="16"/>
       <c r="F32" s="15"/>
       <c r="G32" s="12"/>
       <c r="H32" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="I32" s="15"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="12"/>
+        <v>155</v>
+      </c>
+      <c r="I32" s="142"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="15"/>
       <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="15"/>
       <c r="O32" s="15"/>
       <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
+      <c r="Q32" s="12"/>
       <c r="R32" s="12"/>
       <c r="S32" s="12"/>
-      <c r="T32" s="12"/>
+      <c r="T32" s="30"/>
       <c r="U32" s="30"/>
       <c r="V32" s="30"/>
       <c r="W32" s="30"/>
-      <c r="X32" s="30"/>
-    </row>
-    <row r="33" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
@@ -3744,60 +3590,54 @@
       <c r="F33" s="18"/>
       <c r="G33" s="12"/>
       <c r="H33" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="I33" s="15"/>
-      <c r="J33" s="120" t="s">
-        <v>140</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="I33" s="143"/>
+      <c r="J33" s="15"/>
       <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="12"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="15"/>
       <c r="O33" s="15"/>
       <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
+      <c r="Q33" s="12"/>
       <c r="R33" s="12"/>
       <c r="S33" s="12"/>
-      <c r="T33" s="12"/>
+      <c r="T33" s="30"/>
       <c r="U33" s="30"/>
       <c r="V33" s="30"/>
       <c r="W33" s="30"/>
-      <c r="X33" s="30"/>
-    </row>
-    <row r="34" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
+      <c r="D34" s="15"/>
       <c r="E34" s="12"/>
       <c r="F34" s="18"/>
       <c r="G34" s="18"/>
       <c r="H34" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="I34" s="18"/>
-      <c r="J34" s="120" t="s">
-        <v>148</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="I34" s="143"/>
+      <c r="J34" s="18"/>
       <c r="K34" s="18"/>
       <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="18"/>
       <c r="O34" s="18"/>
       <c r="P34" s="18"/>
       <c r="Q34" s="18"/>
       <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
-      <c r="T34" s="12"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="30"/>
       <c r="U34" s="30"/>
       <c r="V34" s="30"/>
       <c r="W34" s="30"/>
-      <c r="X34" s="30"/>
-    </row>
-    <row r="35" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="75" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -3810,24 +3650,23 @@
       <c r="J35" s="18"/>
       <c r="K35" s="18"/>
       <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="15"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="18"/>
       <c r="Q35" s="18"/>
       <c r="R35" s="18"/>
-      <c r="S35" s="18"/>
-      <c r="T35" s="12"/>
+      <c r="S35" s="12"/>
+      <c r="T35" s="30"/>
       <c r="U35" s="30"/>
       <c r="V35" s="30"/>
       <c r="W35" s="30"/>
-      <c r="X35" s="30"/>
-    </row>
-    <row r="36" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="70"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
-      <c r="D36" s="15"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="12"/>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
@@ -3842,30 +3681,27 @@
       <c r="P36" s="15"/>
       <c r="Q36" s="15"/>
       <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
-      <c r="T36" s="12"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="30"/>
       <c r="U36" s="30"/>
       <c r="V36" s="30"/>
       <c r="W36" s="30"/>
-      <c r="X36" s="30"/>
-    </row>
-    <row r="37" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="136" t="s">
-        <v>160</v>
+    </row>
+    <row r="37" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="131" t="s">
+        <v>153</v>
       </c>
       <c r="B37" s="18"/>
       <c r="C37" s="15"/>
-      <c r="D37" s="18"/>
+      <c r="D37" s="15"/>
       <c r="E37" s="12"/>
       <c r="F37" s="18"/>
       <c r="G37" s="15"/>
       <c r="H37" s="89" t="s">
-        <v>101</v>
-      </c>
-      <c r="I37" s="15"/>
-      <c r="J37" s="92" t="s">
-        <v>123</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="I37" s="12"/>
+      <c r="J37" s="15"/>
       <c r="K37" s="15"/>
       <c r="L37" s="15"/>
       <c r="M37" s="15"/>
@@ -3874,30 +3710,27 @@
       <c r="P37" s="15"/>
       <c r="Q37" s="15"/>
       <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
-      <c r="T37" s="12"/>
+      <c r="S37" s="12"/>
+      <c r="T37" s="30"/>
       <c r="U37" s="30"/>
       <c r="V37" s="30"/>
       <c r="W37" s="30"/>
-      <c r="X37" s="30"/>
-    </row>
-    <row r="38" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="136" t="s">
-        <v>165</v>
+    </row>
+    <row r="38" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="131" t="s">
+        <v>158</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
+      <c r="D38" s="18"/>
       <c r="E38" s="12"/>
       <c r="F38" s="18"/>
       <c r="G38" s="15"/>
-      <c r="H38" s="122" t="s">
-        <v>23</v>
-      </c>
-      <c r="I38" s="15"/>
-      <c r="J38" s="36" t="s">
-        <v>23</v>
-      </c>
+      <c r="H38" s="118" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38" s="12"/>
+      <c r="J38" s="15"/>
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
@@ -3907,13 +3740,12 @@
       <c r="Q38" s="15"/>
       <c r="R38" s="15"/>
       <c r="S38" s="15"/>
-      <c r="T38" s="15"/>
+      <c r="T38" s="30"/>
       <c r="U38" s="30"/>
       <c r="V38" s="30"/>
       <c r="W38" s="30"/>
-      <c r="X38" s="30"/>
-    </row>
-    <row r="39" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="73"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -3922,12 +3754,10 @@
       <c r="F39" s="18"/>
       <c r="G39" s="15"/>
       <c r="H39" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="I39" s="15"/>
-      <c r="J39" s="36" t="s">
-        <v>27</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="I39" s="12"/>
+      <c r="J39" s="15"/>
       <c r="K39" s="15"/>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
@@ -3937,13 +3767,12 @@
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
       <c r="S39" s="15"/>
-      <c r="T39" s="15"/>
+      <c r="T39" s="30"/>
       <c r="U39" s="30"/>
       <c r="V39" s="30"/>
       <c r="W39" s="30"/>
-      <c r="X39" s="30"/>
-    </row>
-    <row r="40" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -3952,10 +3781,10 @@
       <c r="F40" s="18"/>
       <c r="G40" s="15"/>
       <c r="H40" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="I40" s="15"/>
-      <c r="J40" s="18"/>
+        <v>26</v>
+      </c>
+      <c r="I40" s="18"/>
+      <c r="J40" s="15"/>
       <c r="K40" s="15"/>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
@@ -3965,15 +3794,14 @@
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
       <c r="S40" s="15"/>
-      <c r="T40" s="15"/>
+      <c r="T40" s="30"/>
       <c r="U40" s="30"/>
       <c r="V40" s="30"/>
       <c r="W40" s="30"/>
-      <c r="X40" s="30"/>
-    </row>
-    <row r="41" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="75" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -3982,8 +3810,8 @@
       <c r="F41" s="18"/>
       <c r="G41" s="15"/>
       <c r="H41" s="12"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="15"/>
       <c r="K41" s="15"/>
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
@@ -3993,13 +3821,12 @@
       <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
       <c r="S41" s="15"/>
-      <c r="T41" s="15"/>
+      <c r="T41" s="30"/>
       <c r="U41" s="30"/>
       <c r="V41" s="30"/>
       <c r="W41" s="30"/>
-      <c r="X41" s="30"/>
-    </row>
-    <row r="42" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="70"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -4008,10 +3835,8 @@
       <c r="F42" s="18"/>
       <c r="G42" s="15"/>
       <c r="H42" s="12"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="92" t="s">
-        <v>129</v>
-      </c>
+      <c r="I42" s="143"/>
+      <c r="J42" s="15"/>
       <c r="K42" s="15"/>
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
@@ -4021,15 +3846,14 @@
       <c r="Q42" s="15"/>
       <c r="R42" s="15"/>
       <c r="S42" s="15"/>
-      <c r="T42" s="15"/>
+      <c r="T42" s="30"/>
       <c r="U42" s="30"/>
       <c r="V42" s="30"/>
       <c r="W42" s="30"/>
-      <c r="X42" s="30"/>
-    </row>
-    <row r="43" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="136" t="s">
-        <v>138</v>
+    </row>
+    <row r="43" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="131" t="s">
+        <v>133</v>
       </c>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -4038,66 +3862,59 @@
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="36"/>
-      <c r="K43" s="15"/>
+      <c r="I43" s="142"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="18"/>
       <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
+      <c r="M43" s="15"/>
       <c r="N43" s="15"/>
       <c r="O43" s="15"/>
       <c r="P43" s="15"/>
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
       <c r="S43" s="15"/>
-      <c r="T43" s="15"/>
+      <c r="T43" s="30"/>
       <c r="U43" s="30"/>
       <c r="V43" s="30"/>
       <c r="W43" s="30"/>
-      <c r="X43" s="30"/>
-    </row>
-    <row r="44" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="136" t="s">
-        <v>165</v>
+    </row>
+    <row r="44" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="131" t="s">
+        <v>158</v>
       </c>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
-      <c r="D44" s="18"/>
+      <c r="D44" s="15"/>
       <c r="E44" s="15"/>
       <c r="F44" s="15"/>
       <c r="G44" s="15"/>
       <c r="H44" s="12"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="120" t="s">
-        <v>141</v>
-      </c>
-      <c r="K44" s="15"/>
+      <c r="I44" s="143"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="18"/>
       <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
+      <c r="M44" s="15"/>
       <c r="N44" s="15"/>
       <c r="O44" s="15"/>
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
       <c r="S44" s="15"/>
-      <c r="T44" s="15"/>
+      <c r="T44" s="30"/>
       <c r="U44" s="30"/>
       <c r="V44" s="30"/>
       <c r="W44" s="30"/>
-      <c r="X44" s="30"/>
-    </row>
-    <row r="45" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
+      <c r="D45" s="12"/>
       <c r="E45" s="15"/>
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
       <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="120" t="s">
-        <v>148</v>
-      </c>
+      <c r="J45" s="15"/>
       <c r="K45" s="15"/>
       <c r="L45" s="15"/>
       <c r="M45" s="15"/>
@@ -4107,13 +3924,12 @@
       <c r="Q45" s="15"/>
       <c r="R45" s="15"/>
       <c r="S45" s="15"/>
-      <c r="T45" s="15"/>
+      <c r="T45" s="30"/>
       <c r="U45" s="30"/>
       <c r="V45" s="30"/>
       <c r="W45" s="30"/>
-      <c r="X45" s="30"/>
-    </row>
-    <row r="46" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="15"/>
       <c r="C46" s="12"/>
@@ -4122,7 +3938,7 @@
       <c r="F46" s="12"/>
       <c r="G46" s="15"/>
       <c r="H46" s="12"/>
-      <c r="I46" s="18"/>
+      <c r="I46" s="142"/>
       <c r="J46" s="15"/>
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
@@ -4130,18 +3946,17 @@
       <c r="N46" s="15"/>
       <c r="O46" s="15"/>
       <c r="P46" s="15"/>
-      <c r="Q46" s="15"/>
-      <c r="R46" s="12"/>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="15"/>
       <c r="S46" s="15"/>
-      <c r="T46" s="15"/>
+      <c r="T46" s="30"/>
       <c r="U46" s="30"/>
       <c r="V46" s="30"/>
       <c r="W46" s="30"/>
-      <c r="X46" s="30"/>
-    </row>
-    <row r="47" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="75" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
@@ -4161,13 +3976,12 @@
       <c r="Q47" s="12"/>
       <c r="R47" s="12"/>
       <c r="S47" s="12"/>
-      <c r="T47" s="12"/>
+      <c r="T47" s="30"/>
       <c r="U47" s="30"/>
       <c r="V47" s="30"/>
       <c r="W47" s="30"/>
-      <c r="X47" s="30"/>
-    </row>
-    <row r="48" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="70"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
@@ -4187,15 +4001,14 @@
       <c r="Q48" s="12"/>
       <c r="R48" s="12"/>
       <c r="S48" s="12"/>
-      <c r="T48" s="12"/>
+      <c r="T48" s="30"/>
       <c r="U48" s="30"/>
       <c r="V48" s="30"/>
       <c r="W48" s="30"/>
-      <c r="X48" s="30"/>
-    </row>
-    <row r="49" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="136" t="s">
-        <v>144</v>
+    </row>
+    <row r="49" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="131" t="s">
+        <v>138</v>
       </c>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
@@ -4215,15 +4028,14 @@
       <c r="Q49" s="12"/>
       <c r="R49" s="12"/>
       <c r="S49" s="12"/>
-      <c r="T49" s="12"/>
+      <c r="T49" s="30"/>
       <c r="U49" s="30"/>
       <c r="V49" s="30"/>
       <c r="W49" s="30"/>
-      <c r="X49" s="30"/>
-    </row>
-    <row r="50" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="136" t="s">
-        <v>165</v>
+    </row>
+    <row r="50" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="131" t="s">
+        <v>158</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
@@ -4243,15 +4055,14 @@
       <c r="Q50" s="12"/>
       <c r="R50" s="12"/>
       <c r="S50" s="12"/>
-      <c r="T50" s="12"/>
+      <c r="T50" s="30"/>
       <c r="U50" s="30"/>
       <c r="V50" s="30"/>
       <c r="W50" s="30"/>
-      <c r="X50" s="30"/>
-    </row>
-    <row r="51" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="70" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
@@ -4271,15 +4082,14 @@
       <c r="Q51" s="12"/>
       <c r="R51" s="12"/>
       <c r="S51" s="12"/>
-      <c r="T51" s="12"/>
+      <c r="T51" s="30"/>
       <c r="U51" s="30"/>
       <c r="V51" s="30"/>
       <c r="W51" s="30"/>
-      <c r="X51" s="30"/>
-    </row>
-    <row r="52" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="70" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
@@ -4299,29 +4109,28 @@
       <c r="Q52" s="12"/>
       <c r="R52" s="12"/>
       <c r="S52" s="12"/>
-      <c r="T52" s="12"/>
+      <c r="T52" s="30"/>
       <c r="U52" s="30"/>
       <c r="V52" s="30"/>
       <c r="W52" s="30"/>
-      <c r="X52" s="30"/>
-    </row>
-    <row r="53" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U53" s="30"/>
       <c r="V53" s="30"/>
       <c r="W53" s="30"/>
       <c r="X53" s="30"/>
-      <c r="Y53" s="30"/>
-    </row>
-    <row r="54" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="54" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5260,8 +5069,8 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="V1:AI1"/>
-    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="U1:AH1"/>
+    <mergeCell ref="A1:S1"/>
   </mergeCells>
   <conditionalFormatting sqref="A47 A41:A42 A35:A36 A32 A29">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
@@ -5303,22 +5112,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="146" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="146"/>
-      <c r="K1" s="146"/>
-      <c r="L1" s="146"/>
-      <c r="M1" s="146"/>
-      <c r="N1" s="146"/>
+      <c r="A1" s="141" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="141"/>
       <c r="O1" s="64"/>
       <c r="P1" s="57"/>
       <c r="Q1" s="57"/>
@@ -5331,25 +5140,25 @@
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2" s="52" t="s">
+        <v>172</v>
+      </c>
+      <c r="G2" s="51" t="s">
         <v>173</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" s="49" t="s">
-        <v>175</v>
-      </c>
-      <c r="D2" s="50" t="s">
-        <v>176</v>
-      </c>
-      <c r="E2" s="51" t="s">
-        <v>178</v>
-      </c>
-      <c r="F2" s="52" t="s">
-        <v>179</v>
-      </c>
-      <c r="G2" s="51" t="s">
-        <v>180</v>
       </c>
       <c r="H2" s="53" t="s">
         <v>5</v>
@@ -5358,19 +5167,19 @@
         <v>4</v>
       </c>
       <c r="J2" s="54" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K2" s="54" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L2" s="55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M2" s="61" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N2" s="65" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="O2" s="63"/>
       <c r="P2" s="58"/>
@@ -5384,46 +5193,46 @@
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" s="43" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>186</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>187</v>
-      </c>
-      <c r="G3" s="43" t="s">
-        <v>188</v>
-      </c>
       <c r="H3" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M3" s="62" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N3" s="66" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="O3" s="28"/>
       <c r="P3" s="28"/>
@@ -5437,44 +5246,44 @@
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="F4" s="44" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="G4" s="43" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M4" s="62" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="N4" s="66" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="O4" s="28"/>
       <c r="P4" s="28"/>
@@ -5488,42 +5297,42 @@
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="E5" s="43"/>
       <c r="F5" s="43"/>
       <c r="G5" s="43" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M5" s="62" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="N5" s="66" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="O5" s="28"/>
       <c r="P5" s="28"/>
@@ -5538,34 +5347,34 @@
     <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
       <c r="G6" s="43" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M6" s="62" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N6" s="67"/>
       <c r="O6" s="28"/>
@@ -5581,30 +5390,30 @@
     <row r="7" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="43"/>
       <c r="F7" s="43"/>
       <c r="G7" s="43"/>
       <c r="H7" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="16" t="s">
         <v>70</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>73</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="15" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="M7" s="62" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="N7" s="67"/>
       <c r="O7" s="28"/>
@@ -5620,27 +5429,27 @@
     <row r="8" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="43"/>
       <c r="F8" s="43"/>
       <c r="G8" s="43"/>
       <c r="H8" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="15" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M8" s="56"/>
       <c r="N8" s="67"/>
@@ -5663,17 +5472,17 @@
       <c r="F9" s="43"/>
       <c r="G9" s="43"/>
       <c r="H9" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="15" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="M9" s="56"/>
       <c r="N9" s="67"/>
@@ -5696,15 +5505,15 @@
       <c r="F10" s="43"/>
       <c r="G10" s="43"/>
       <c r="H10" s="22" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="16" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="L10" s="24" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="M10" s="56"/>
       <c r="N10" s="67"/>
@@ -5721,12 +5530,12 @@
     <row r="11" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="9"/>
       <c r="E11" s="46" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="F11" s="43"/>
       <c r="G11" s="43"/>
@@ -5750,12 +5559,12 @@
     <row r="12" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="9"/>
       <c r="E12" s="43" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F12" s="43"/>
       <c r="G12" s="43"/>
@@ -5779,12 +5588,12 @@
     <row r="13" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="9"/>
       <c r="E13" s="43" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="F13" s="43"/>
       <c r="G13" s="43"/>
@@ -5811,7 +5620,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="9"/>
       <c r="E14" s="43" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F14" s="43"/>
       <c r="G14" s="43"/>
@@ -5878,20 +5687,20 @@
     <row r="18" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="4" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D18" s="8"/>
       <c r="N18" s="6" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="P18" s="59"/>
     </row>
     <row r="19" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N19" s="7" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="P19" s="59"/>
     </row>

</xml_diff>